<commit_message>
cat user role root
</commit_message>
<xml_diff>
--- a/Document/4.Test/180721_DeXuatSua.xlsx
+++ b/Document/4.Test/180721_DeXuatSua.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20228"/>
   <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E09AA43-C642-4923-BF15-BD469D2C6444}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="45">
   <si>
     <t>TT</t>
   </si>
@@ -167,16 +168,22 @@
 2. Cho phép auto suggesstion theo cả tên hang hóa
 3. Bổ sung cột Thành tiền ở phần danh sách hàng hóa và lable tổng tiền cạnh ô tìm kiếm nhanh</t>
   </si>
+  <si>
+    <t>Resolve</t>
+  </si>
+  <si>
+    <t>Confirm</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -184,7 +191,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -556,26 +563,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="6" customWidth="1"/>
-    <col min="2" max="2" width="17.75" customWidth="1"/>
-    <col min="3" max="3" width="19.25" customWidth="1"/>
-    <col min="4" max="4" width="9.875" customWidth="1"/>
-    <col min="5" max="5" width="47.375" customWidth="1"/>
-    <col min="6" max="6" width="54.875" customWidth="1"/>
-    <col min="7" max="8" width="12.25" customWidth="1"/>
-    <col min="9" max="9" width="9.25" customWidth="1"/>
+    <col min="2" max="2" width="17.7265625" customWidth="1"/>
+    <col min="3" max="3" width="19.26953125" customWidth="1"/>
+    <col min="4" max="4" width="9.90625" customWidth="1"/>
+    <col min="5" max="5" width="47.36328125" customWidth="1"/>
+    <col min="6" max="6" width="54.90625" customWidth="1"/>
+    <col min="7" max="8" width="12.26953125" customWidth="1"/>
+    <col min="9" max="9" width="9.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -604,7 +611,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="85.5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" ht="87" x14ac:dyDescent="0.35">
       <c r="A2" s="5">
         <v>1</v>
       </c>
@@ -633,7 +640,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A3" s="5">
         <v>2</v>
       </c>
@@ -662,7 +669,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="57" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" ht="58" x14ac:dyDescent="0.35">
       <c r="A4" s="5">
         <v>3</v>
       </c>
@@ -688,10 +695,10 @@
         <v>15</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="28.5" x14ac:dyDescent="0.2">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A5" s="5">
         <v>4</v>
       </c>
@@ -717,10 +724,10 @@
         <v>15</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="85.5" x14ac:dyDescent="0.2">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="87" x14ac:dyDescent="0.35">
       <c r="A6" s="5">
         <v>5</v>
       </c>
@@ -746,10 +753,10 @@
         <v>15</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="28.5" x14ac:dyDescent="0.2">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A7" s="5">
         <v>6</v>
       </c>
@@ -776,7 +783,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="57" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" ht="58" x14ac:dyDescent="0.35">
       <c r="A8" s="5">
         <v>7</v>
       </c>
@@ -805,7 +812,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A9" s="5"/>
       <c r="B9" s="3" t="s">
         <v>36</v>
@@ -832,7 +839,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="71.25" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A10" s="5"/>
       <c r="B10" s="3" t="s">
         <v>40</v>
@@ -859,7 +866,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" s="5"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
@@ -870,7 +877,7 @@
       <c r="H11" s="3"/>
       <c r="I11" s="3"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" s="5"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
@@ -881,7 +888,7 @@
       <c r="H12" s="3"/>
       <c r="I12" s="3"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" s="5"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
@@ -892,7 +899,7 @@
       <c r="H13" s="3"/>
       <c r="I13" s="3"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" s="5"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
@@ -903,7 +910,7 @@
       <c r="H14" s="3"/>
       <c r="I14" s="3"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" s="5"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
@@ -914,7 +921,7 @@
       <c r="H15" s="3"/>
       <c r="I15" s="3"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" s="5"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
@@ -925,7 +932,7 @@
       <c r="H16" s="3"/>
       <c r="I16" s="3"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17" s="5"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
@@ -936,7 +943,7 @@
       <c r="H17" s="3"/>
       <c r="I17" s="3"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18" s="5"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
@@ -947,7 +954,7 @@
       <c r="H18" s="3"/>
       <c r="I18" s="3"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19" s="5"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
@@ -958,7 +965,7 @@
       <c r="H19" s="3"/>
       <c r="I19" s="3"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20" s="5"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
@@ -969,7 +976,7 @@
       <c r="H20" s="3"/>
       <c r="I20" s="3"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21" s="5"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
@@ -980,7 +987,7 @@
       <c r="H21" s="3"/>
       <c r="I21" s="3"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A22" s="5"/>
       <c r="B22" s="7"/>
       <c r="C22" s="7"/>
@@ -991,7 +998,7 @@
       <c r="H22" s="6"/>
       <c r="I22" s="3"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23" s="5"/>
       <c r="B23" s="7"/>
       <c r="C23" s="7"/>
@@ -1002,7 +1009,7 @@
       <c r="H23" s="6"/>
       <c r="I23" s="3"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A24" s="5"/>
       <c r="B24" s="7"/>
       <c r="C24" s="7"/>
@@ -1013,7 +1020,7 @@
       <c r="H24" s="6"/>
       <c r="I24" s="3"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A25" s="5"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
@@ -1024,7 +1031,7 @@
       <c r="H25" s="3"/>
       <c r="I25" s="3"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A26" s="5"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
@@ -1035,7 +1042,7 @@
       <c r="H26" s="6"/>
       <c r="I26" s="3"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A27" s="5"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
@@ -1046,7 +1053,7 @@
       <c r="H27" s="6"/>
       <c r="I27" s="3"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A28" s="5"/>
       <c r="B28" s="3"/>
       <c r="C28" s="7"/>
@@ -1057,7 +1064,7 @@
       <c r="H28" s="6"/>
       <c r="I28" s="3"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A29" s="5"/>
       <c r="B29" s="7"/>
       <c r="C29" s="7"/>
@@ -1068,7 +1075,7 @@
       <c r="H29" s="6"/>
       <c r="I29" s="3"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A30" s="5"/>
       <c r="B30" s="7"/>
       <c r="C30" s="7"/>
@@ -1079,7 +1086,7 @@
       <c r="H30" s="6"/>
       <c r="I30" s="3"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A31" s="5"/>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
@@ -1090,7 +1097,7 @@
       <c r="H31" s="6"/>
       <c r="I31" s="3"/>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A32" s="5"/>
       <c r="B32" s="7"/>
       <c r="C32" s="7"/>
@@ -1101,7 +1108,7 @@
       <c r="H32" s="6"/>
       <c r="I32" s="3"/>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A33" s="5"/>
       <c r="B33" s="7"/>
       <c r="C33" s="7"/>
@@ -1112,7 +1119,7 @@
       <c r="H33" s="6"/>
       <c r="I33" s="3"/>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A34" s="5"/>
       <c r="B34" s="9"/>
       <c r="C34" s="10"/>
@@ -1123,7 +1130,7 @@
       <c r="H34" s="6"/>
       <c r="I34" s="3"/>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A35" s="5"/>
       <c r="B35" s="9"/>
       <c r="C35" s="10"/>
@@ -1134,7 +1141,7 @@
       <c r="H35" s="6"/>
       <c r="I35" s="3"/>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A36" s="5"/>
       <c r="B36" s="9"/>
       <c r="C36" s="10"/>
@@ -1145,7 +1152,7 @@
       <c r="H36" s="6"/>
       <c r="I36" s="3"/>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A37" s="5"/>
       <c r="B37" s="9"/>
       <c r="C37" s="10"/>
@@ -1156,7 +1163,7 @@
       <c r="H37" s="6"/>
       <c r="I37" s="3"/>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A38" s="5"/>
       <c r="B38" s="9"/>
       <c r="C38" s="10"/>
@@ -1167,7 +1174,7 @@
       <c r="H38" s="6"/>
       <c r="I38" s="3"/>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A39" s="5"/>
       <c r="B39" s="9"/>
       <c r="C39" s="10"/>
@@ -1178,7 +1185,7 @@
       <c r="H39" s="6"/>
       <c r="I39" s="3"/>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A40" s="5"/>
       <c r="B40" s="9"/>
       <c r="C40" s="9"/>
@@ -1189,7 +1196,7 @@
       <c r="H40" s="6"/>
       <c r="I40" s="3"/>
     </row>
-    <row r="41" spans="1:9" ht="79.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:9" ht="79.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A41" s="5"/>
       <c r="B41" s="9"/>
       <c r="C41" s="9"/>
@@ -1200,7 +1207,7 @@
       <c r="H41" s="6"/>
       <c r="I41" s="3"/>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A42" s="5"/>
       <c r="B42" s="10"/>
       <c r="C42" s="10"/>
@@ -1211,7 +1218,7 @@
       <c r="H42" s="6"/>
       <c r="I42" s="3"/>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A43" s="5"/>
       <c r="B43" s="10"/>
       <c r="C43" s="10"/>
@@ -1222,7 +1229,7 @@
       <c r="H43" s="6"/>
       <c r="I43" s="3"/>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A44" s="5"/>
       <c r="B44" s="10"/>
       <c r="C44" s="10"/>
@@ -1233,7 +1240,7 @@
       <c r="H44" s="6"/>
       <c r="I44" s="3"/>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A45" s="5"/>
       <c r="B45" s="10"/>
       <c r="C45" s="10"/>
@@ -1244,7 +1251,7 @@
       <c r="H45" s="6"/>
       <c r="I45" s="3"/>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A46" s="5"/>
       <c r="B46" s="10"/>
       <c r="C46" s="10"/>
@@ -1255,7 +1262,7 @@
       <c r="H46" s="6"/>
       <c r="I46" s="3"/>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A47" s="5"/>
       <c r="B47" s="9"/>
       <c r="C47" s="10"/>
@@ -1266,7 +1273,7 @@
       <c r="H47" s="6"/>
       <c r="I47" s="3"/>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A48" s="5"/>
       <c r="B48" s="9"/>
       <c r="C48" s="10"/>
@@ -1277,7 +1284,7 @@
       <c r="H48" s="6"/>
       <c r="I48" s="3"/>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A49" s="5"/>
       <c r="B49" s="9"/>
       <c r="C49" s="10"/>
@@ -1288,7 +1295,7 @@
       <c r="H49" s="6"/>
       <c r="I49" s="3"/>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A50" s="5"/>
       <c r="B50" s="9"/>
       <c r="C50" s="10"/>
@@ -1299,7 +1306,7 @@
       <c r="H50" s="6"/>
       <c r="I50" s="3"/>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A51" s="5"/>
       <c r="B51" s="9"/>
       <c r="C51" s="10"/>
@@ -1310,7 +1317,7 @@
       <c r="H51" s="6"/>
       <c r="I51" s="3"/>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A52" s="5"/>
       <c r="B52" s="9"/>
       <c r="C52" s="10"/>
@@ -1321,7 +1328,7 @@
       <c r="H52" s="6"/>
       <c r="I52" s="3"/>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A53" s="5"/>
       <c r="B53" s="9"/>
       <c r="C53" s="10"/>
@@ -1332,7 +1339,7 @@
       <c r="H53" s="6"/>
       <c r="I53" s="3"/>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A54" s="5"/>
       <c r="B54" s="9"/>
       <c r="C54" s="10"/>
@@ -1343,7 +1350,7 @@
       <c r="H54" s="6"/>
       <c r="I54" s="3"/>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A55" s="5"/>
       <c r="B55" s="9"/>
       <c r="C55" s="10"/>
@@ -1354,7 +1361,7 @@
       <c r="H55" s="6"/>
       <c r="I55" s="3"/>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A56" s="5"/>
       <c r="B56" s="9"/>
       <c r="C56" s="10"/>
@@ -1365,7 +1372,7 @@
       <c r="H56" s="6"/>
       <c r="I56" s="3"/>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A57" s="5"/>
       <c r="B57" s="9"/>
       <c r="C57" s="9"/>
@@ -1376,7 +1383,7 @@
       <c r="H57" s="6"/>
       <c r="I57" s="3"/>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A58" s="1"/>
       <c r="B58" s="9"/>
       <c r="C58" s="10"/>
@@ -1387,7 +1394,7 @@
       <c r="H58" s="6"/>
       <c r="I58" s="3"/>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A59" s="1"/>
       <c r="B59" s="9"/>
       <c r="C59" s="10"/>
@@ -1399,12 +1406,12 @@
       <c r="I59" s="3"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I59"/>
+  <autoFilter ref="A1:I59" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I1048576" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"New, Resolve, Confirm, Close, Cancel, Accept"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"Lỗi, Đề xuất"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Doan day danh sach loi
</commit_message>
<xml_diff>
--- a/Document/4.Test/180721_DeXuatSua.xlsx
+++ b/Document/4.Test/180721_DeXuatSua.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E043A6C0-31ED-4469-AF4E-E8A582E7853B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="57">
   <si>
     <t>TT</t>
   </si>
@@ -155,11 +156,6 @@
     <t>1. Khi thay đổi kho thì combobox vị trí của Kho không thay đổi theo.
 2. Nếu không nhớ mã hàng hóa thì không thể nhập được kho
 3. Không hiển thị được tổng giá trị của 1 lần nhập kho</t>
-  </si>
-  <si>
-    <t>1. Khi thay đổi kho thì combobox vị trí của Kho thay đổi theo.
-2. Cho phép auto suggesstion theo cả tên hàng hóa
-3. Bổ sung cột Thành tiền ở phần danh sách hàng hóa và lable Tổng tiền cạnh ô tìm kiếm nhanh.</t>
   </si>
   <si>
     <t>1. Bỏ cột Trạng thái
@@ -222,7 +218,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FF00B050"/>
-        <rFont val="Arial"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="163"/>
         <scheme val="minor"/>
@@ -233,7 +229,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Arial"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -244,7 +240,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FF00B050"/>
-        <rFont val="Arial"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -254,7 +250,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Arial"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -265,7 +261,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FF00B050"/>
-        <rFont val="Arial"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <charset val="163"/>
         <scheme val="minor"/>
@@ -276,7 +272,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Arial"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -284,16 +280,78 @@
 4. Khi xem thông tin giao dịch hiển thị các trường khác như Đối tác nhận, người xuất, ngày xuất, kho xuất…</t>
     </r>
   </si>
+  <si>
+    <t>Confirm</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1. Khi thay đổi kho thì combobox vị trí của Kho thay đổi theo </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>=&gt; OK</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+2. Cho phép auto suggesstion theo cả tên hàng hóa </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>=&gt; OK</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+3. Bổ sung cột Thành tiền ở phần danh sách hàng hóa và lable Tổng tiền cạnh ô tìm kiếm nhanh </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>=&gt; OK (chỉnh ra căn phải hợp lý hơn)</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -301,23 +359,31 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF00B050"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF00B050"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="163"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -711,24 +777,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I59"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6" customWidth="1"/>
-    <col min="2" max="2" width="17.75" customWidth="1"/>
-    <col min="3" max="3" width="19.25" customWidth="1"/>
-    <col min="4" max="4" width="9.875" customWidth="1"/>
-    <col min="5" max="5" width="41.125" customWidth="1"/>
-    <col min="6" max="6" width="54.875" customWidth="1"/>
-    <col min="7" max="8" width="12.25" customWidth="1"/>
-    <col min="9" max="9" width="9.25" customWidth="1"/>
+    <col min="2" max="2" width="17.7109375" customWidth="1"/>
+    <col min="3" max="3" width="19.28515625" customWidth="1"/>
+    <col min="4" max="4" width="9.85546875" customWidth="1"/>
+    <col min="5" max="5" width="41.140625" customWidth="1"/>
+    <col min="6" max="6" width="54.85546875" customWidth="1"/>
+    <col min="7" max="8" width="12.28515625" customWidth="1"/>
+    <col min="9" max="9" width="9.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -760,65 +825,65 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="85.5" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="5">
+    <row r="2" spans="1:9" ht="105" x14ac:dyDescent="0.25">
+      <c r="A2" s="13">
         <v>1</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="G2" s="6">
+      <c r="G2" s="16">
         <v>43302</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="H2" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="I2" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="42.75" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="5">
+      <c r="I2" s="14" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="13">
         <v>2</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="F3" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="G3" s="6">
+      <c r="G3" s="16">
         <v>43302</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="H3" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="I3" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="78" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I3" s="14" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="78" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <v>3</v>
       </c>
@@ -844,10 +909,10 @@
         <v>15</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="47.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="13">
         <v>4</v>
       </c>
@@ -873,66 +938,66 @@
         <v>15</v>
       </c>
       <c r="I5" s="14" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="99.75" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="5">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="105" x14ac:dyDescent="0.25">
+      <c r="A6" s="13">
         <v>5</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="E6" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="F6" s="4" t="s">
+      <c r="F6" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="G6" s="6">
+      <c r="G6" s="16">
         <v>43302</v>
       </c>
-      <c r="H6" s="3" t="s">
+      <c r="H6" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="I6" s="3" t="s">
+      <c r="I6" s="14" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="13">
         <v>6</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" ht="28.5" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="5">
-        <v>6</v>
-      </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D7" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4" t="s">
+      <c r="E7" s="15"/>
+      <c r="F7" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="G7" s="6">
+      <c r="G7" s="16">
         <v>43302</v>
       </c>
-      <c r="H7" s="6" t="s">
+      <c r="H7" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="I7" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" ht="71.25" x14ac:dyDescent="0.2">
+      <c r="I7" s="14" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
         <v>7</v>
       </c>
@@ -949,7 +1014,7 @@
         <v>33</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G8" s="6">
         <v>43302</v>
@@ -961,82 +1026,82 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="28.5" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="5">
+    <row r="9" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="13">
         <v>8</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="D9" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="E9" s="3" t="s">
+      <c r="E9" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="F9" s="3" t="s">
+      <c r="F9" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="G9" s="6">
+      <c r="G9" s="16">
         <v>43302</v>
       </c>
-      <c r="H9" s="6" t="s">
+      <c r="H9" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="I9" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="85.5" x14ac:dyDescent="0.2">
-      <c r="A10" s="5">
+      <c r="I9" s="14" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+      <c r="A10" s="13">
         <v>9</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="D10" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="E10" s="3" t="s">
+      <c r="E10" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="F10" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="G10" s="6">
+      <c r="F10" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="G10" s="16">
         <v>43302</v>
       </c>
-      <c r="H10" s="6" t="s">
+      <c r="H10" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="I10" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="71.25" x14ac:dyDescent="0.2">
+      <c r="I10" s="14" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="75" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
         <v>10</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E11" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="F11" s="3" t="s">
         <v>44</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>45</v>
       </c>
       <c r="G11" s="6">
         <v>43302</v>
@@ -1048,24 +1113,24 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="114" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" ht="120" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
         <v>11</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>3</v>
       </c>
       <c r="E12" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="F12" s="3" t="s">
         <v>52</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>53</v>
       </c>
       <c r="G12" s="6">
         <v>43302</v>
@@ -1077,24 +1142,24 @@
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="99.75" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" ht="120" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
         <v>12</v>
       </c>
       <c r="B13" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C13" s="3" t="s">
         <v>46</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>47</v>
       </c>
       <c r="D13" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G13" s="6">
         <v>43302</v>
@@ -1106,24 +1171,24 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="99.75" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
         <v>13</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G14" s="6">
         <v>43302</v>
@@ -1135,7 +1200,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="5"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
@@ -1146,7 +1211,7 @@
       <c r="H15" s="3"/>
       <c r="I15" s="3"/>
     </row>
-    <row r="16" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="5"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
@@ -1157,7 +1222,7 @@
       <c r="H16" s="3"/>
       <c r="I16" s="3"/>
     </row>
-    <row r="17" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="5"/>
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
@@ -1168,7 +1233,7 @@
       <c r="H17" s="3"/>
       <c r="I17" s="3"/>
     </row>
-    <row r="18" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="5"/>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
@@ -1179,7 +1244,7 @@
       <c r="H18" s="3"/>
       <c r="I18" s="3"/>
     </row>
-    <row r="19" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="5"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
@@ -1190,7 +1255,7 @@
       <c r="H19" s="3"/>
       <c r="I19" s="3"/>
     </row>
-    <row r="20" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="5"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
@@ -1201,7 +1266,7 @@
       <c r="H20" s="3"/>
       <c r="I20" s="3"/>
     </row>
-    <row r="21" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="5"/>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
@@ -1212,7 +1277,7 @@
       <c r="H21" s="3"/>
       <c r="I21" s="3"/>
     </row>
-    <row r="22" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="5"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
@@ -1223,7 +1288,7 @@
       <c r="H22" s="3"/>
       <c r="I22" s="3"/>
     </row>
-    <row r="23" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="5"/>
       <c r="B23" s="7"/>
       <c r="C23" s="7"/>
@@ -1234,7 +1299,7 @@
       <c r="H23" s="6"/>
       <c r="I23" s="3"/>
     </row>
-    <row r="24" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="5"/>
       <c r="B24" s="7"/>
       <c r="C24" s="7"/>
@@ -1245,7 +1310,7 @@
       <c r="H24" s="6"/>
       <c r="I24" s="3"/>
     </row>
-    <row r="25" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="5"/>
       <c r="B25" s="7"/>
       <c r="C25" s="7"/>
@@ -1256,7 +1321,7 @@
       <c r="H25" s="6"/>
       <c r="I25" s="3"/>
     </row>
-    <row r="26" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="5"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
@@ -1267,7 +1332,7 @@
       <c r="H26" s="3"/>
       <c r="I26" s="3"/>
     </row>
-    <row r="27" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="5"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
@@ -1278,7 +1343,7 @@
       <c r="H27" s="6"/>
       <c r="I27" s="3"/>
     </row>
-    <row r="28" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="5"/>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
@@ -1289,7 +1354,7 @@
       <c r="H28" s="6"/>
       <c r="I28" s="3"/>
     </row>
-    <row r="29" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="5"/>
       <c r="B29" s="3"/>
       <c r="C29" s="7"/>
@@ -1300,7 +1365,7 @@
       <c r="H29" s="6"/>
       <c r="I29" s="3"/>
     </row>
-    <row r="30" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="5"/>
       <c r="B30" s="7"/>
       <c r="C30" s="7"/>
@@ -1311,7 +1376,7 @@
       <c r="H30" s="6"/>
       <c r="I30" s="3"/>
     </row>
-    <row r="31" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="5"/>
       <c r="B31" s="7"/>
       <c r="C31" s="7"/>
@@ -1322,7 +1387,7 @@
       <c r="H31" s="6"/>
       <c r="I31" s="3"/>
     </row>
-    <row r="32" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="5"/>
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
@@ -1333,7 +1398,7 @@
       <c r="H32" s="6"/>
       <c r="I32" s="3"/>
     </row>
-    <row r="33" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="5"/>
       <c r="B33" s="7"/>
       <c r="C33" s="7"/>
@@ -1344,7 +1409,7 @@
       <c r="H33" s="6"/>
       <c r="I33" s="3"/>
     </row>
-    <row r="34" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="5"/>
       <c r="B34" s="7"/>
       <c r="C34" s="7"/>
@@ -1355,7 +1420,7 @@
       <c r="H34" s="6"/>
       <c r="I34" s="3"/>
     </row>
-    <row r="35" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="5"/>
       <c r="B35" s="9"/>
       <c r="C35" s="10"/>
@@ -1366,7 +1431,7 @@
       <c r="H35" s="6"/>
       <c r="I35" s="3"/>
     </row>
-    <row r="36" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="5"/>
       <c r="B36" s="9"/>
       <c r="C36" s="10"/>
@@ -1377,7 +1442,7 @@
       <c r="H36" s="6"/>
       <c r="I36" s="3"/>
     </row>
-    <row r="37" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="5"/>
       <c r="B37" s="9"/>
       <c r="C37" s="10"/>
@@ -1388,7 +1453,7 @@
       <c r="H37" s="6"/>
       <c r="I37" s="3"/>
     </row>
-    <row r="38" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="5"/>
       <c r="B38" s="9"/>
       <c r="C38" s="10"/>
@@ -1399,7 +1464,7 @@
       <c r="H38" s="6"/>
       <c r="I38" s="3"/>
     </row>
-    <row r="39" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="5"/>
       <c r="B39" s="9"/>
       <c r="C39" s="10"/>
@@ -1410,7 +1475,7 @@
       <c r="H39" s="6"/>
       <c r="I39" s="3"/>
     </row>
-    <row r="40" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="5"/>
       <c r="B40" s="9"/>
       <c r="C40" s="10"/>
@@ -1421,7 +1486,7 @@
       <c r="H40" s="6"/>
       <c r="I40" s="3"/>
     </row>
-    <row r="41" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="5"/>
       <c r="B41" s="9"/>
       <c r="C41" s="9"/>
@@ -1432,7 +1497,7 @@
       <c r="H41" s="6"/>
       <c r="I41" s="3"/>
     </row>
-    <row r="42" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="5"/>
       <c r="B42" s="10"/>
       <c r="C42" s="10"/>
@@ -1443,7 +1508,7 @@
       <c r="H42" s="6"/>
       <c r="I42" s="3"/>
     </row>
-    <row r="43" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="5"/>
       <c r="B43" s="10"/>
       <c r="C43" s="10"/>
@@ -1454,7 +1519,7 @@
       <c r="H43" s="6"/>
       <c r="I43" s="3"/>
     </row>
-    <row r="44" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="5"/>
       <c r="B44" s="10"/>
       <c r="C44" s="10"/>
@@ -1465,7 +1530,7 @@
       <c r="H44" s="6"/>
       <c r="I44" s="3"/>
     </row>
-    <row r="45" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="5"/>
       <c r="B45" s="10"/>
       <c r="C45" s="10"/>
@@ -1476,7 +1541,7 @@
       <c r="H45" s="6"/>
       <c r="I45" s="3"/>
     </row>
-    <row r="46" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="5"/>
       <c r="B46" s="10"/>
       <c r="C46" s="10"/>
@@ -1487,7 +1552,7 @@
       <c r="H46" s="6"/>
       <c r="I46" s="3"/>
     </row>
-    <row r="47" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="5"/>
       <c r="B47" s="9"/>
       <c r="C47" s="10"/>
@@ -1498,7 +1563,7 @@
       <c r="H47" s="6"/>
       <c r="I47" s="3"/>
     </row>
-    <row r="48" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" s="5"/>
       <c r="B48" s="9"/>
       <c r="C48" s="10"/>
@@ -1509,7 +1574,7 @@
       <c r="H48" s="6"/>
       <c r="I48" s="3"/>
     </row>
-    <row r="49" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" s="5"/>
       <c r="B49" s="9"/>
       <c r="C49" s="10"/>
@@ -1520,7 +1585,7 @@
       <c r="H49" s="6"/>
       <c r="I49" s="3"/>
     </row>
-    <row r="50" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" s="5"/>
       <c r="B50" s="9"/>
       <c r="C50" s="10"/>
@@ -1531,7 +1596,7 @@
       <c r="H50" s="6"/>
       <c r="I50" s="3"/>
     </row>
-    <row r="51" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" s="5"/>
       <c r="B51" s="9"/>
       <c r="C51" s="10"/>
@@ -1542,7 +1607,7 @@
       <c r="H51" s="6"/>
       <c r="I51" s="3"/>
     </row>
-    <row r="52" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" s="5"/>
       <c r="B52" s="9"/>
       <c r="C52" s="10"/>
@@ -1553,7 +1618,7 @@
       <c r="H52" s="6"/>
       <c r="I52" s="3"/>
     </row>
-    <row r="53" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" s="5"/>
       <c r="B53" s="9"/>
       <c r="C53" s="10"/>
@@ -1564,7 +1629,7 @@
       <c r="H53" s="6"/>
       <c r="I53" s="3"/>
     </row>
-    <row r="54" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" s="5"/>
       <c r="B54" s="9"/>
       <c r="C54" s="10"/>
@@ -1575,7 +1640,7 @@
       <c r="H54" s="6"/>
       <c r="I54" s="3"/>
     </row>
-    <row r="55" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" s="5"/>
       <c r="B55" s="9"/>
       <c r="C55" s="10"/>
@@ -1586,7 +1651,7 @@
       <c r="H55" s="6"/>
       <c r="I55" s="3"/>
     </row>
-    <row r="56" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" s="5"/>
       <c r="B56" s="9"/>
       <c r="C56" s="10"/>
@@ -1597,7 +1662,7 @@
       <c r="H56" s="6"/>
       <c r="I56" s="3"/>
     </row>
-    <row r="57" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" s="5"/>
       <c r="B57" s="9"/>
       <c r="C57" s="9"/>
@@ -1608,7 +1673,7 @@
       <c r="H57" s="6"/>
       <c r="I57" s="3"/>
     </row>
-    <row r="58" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" s="1"/>
       <c r="B58" s="9"/>
       <c r="C58" s="10"/>
@@ -1619,7 +1684,7 @@
       <c r="H58" s="6"/>
       <c r="I58" s="3"/>
     </row>
-    <row r="59" spans="1:9" hidden="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" s="1"/>
       <c r="B59" s="9"/>
       <c r="C59" s="10"/>
@@ -1631,18 +1696,12 @@
       <c r="I59" s="3"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I59">
-    <filterColumn colId="7">
-      <filters>
-        <filter val="DuyOT"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:I59" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I1048576" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"New, Resolve, Confirm, Close, Cancel, Accept"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"Lỗi, Đề xuất"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>